<commit_message>
The one we used!
</commit_message>
<xml_diff>
--- a/Real2020Entry1/forBot_StudentRequestList.xlsx
+++ b/Real2020Entry1/forBot_StudentRequestList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/Real2020Entry1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F47FC2-47C2-3645-B103-7212C7DFDBF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B858C0A7-A3FF-6A4B-9406-17BECDE5020C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,7 +626,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>

</xml_diff>